<commit_message>
modify: modify all data(need check twich)
</commit_message>
<xml_diff>
--- a/ALL/All_data_des.xlsx
+++ b/ALL/All_data_des.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -727,175 +727,175 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>858</v>
+        <v>1334</v>
       </c>
       <c r="C2" t="n">
-        <v>781</v>
+        <v>1253</v>
       </c>
       <c r="D2" t="n">
-        <v>809</v>
+        <v>1277</v>
       </c>
       <c r="E2" t="n">
-        <v>804</v>
+        <v>1253</v>
       </c>
       <c r="F2" t="n">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="G2" t="n">
-        <v>241</v>
+        <v>330</v>
       </c>
       <c r="H2" t="n">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="I2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="J2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="K2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="L2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="M2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="N2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="O2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="P2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="Q2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="R2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="S2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="T2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="U2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="V2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="W2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="X2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="Y2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="Z2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AA2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AB2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AC2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AD2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AE2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AF2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AG2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AH2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AI2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AJ2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AK2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AL2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AM2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AN2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AO2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AP2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AQ2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AR2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AS2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AT2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AU2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AV2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AW2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AX2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AY2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="AZ2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="BA2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="BB2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="BC2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="BD2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="BE2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
       <c r="BF2" t="n">
-        <v>1075</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="3">
@@ -905,175 +905,175 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>624.0149184149185</v>
+        <v>621.8589205397302</v>
       </c>
       <c r="C3" t="n">
-        <v>674.657362355954</v>
+        <v>672.6064644852355</v>
       </c>
       <c r="D3" t="n">
-        <v>1073.190160692213</v>
+        <v>1066.580297572435</v>
       </c>
       <c r="E3" t="n">
-        <v>5.892512437810945</v>
+        <v>5.804293695131684</v>
       </c>
       <c r="F3" t="n">
-        <v>1814.35</v>
+        <v>1791.778947368421</v>
       </c>
       <c r="G3" t="n">
-        <v>92.85178423236516</v>
+        <v>92.7741515151515</v>
       </c>
       <c r="H3" t="n">
-        <v>4.110566037735849</v>
+        <v>3.541875</v>
       </c>
       <c r="I3" t="n">
-        <v>7.352710976744185</v>
+        <v>6.786198348623854</v>
       </c>
       <c r="J3" t="n">
-        <v>0.4625348837209302</v>
+        <v>0.466559633027523</v>
       </c>
       <c r="K3" t="n">
-        <v>1.005079069767442</v>
+        <v>0.9783853211009174</v>
       </c>
       <c r="L3" t="n">
-        <v>1.096394418604651</v>
+        <v>1.010491743119266</v>
       </c>
       <c r="M3" t="n">
-        <v>2.324244744186047</v>
+        <v>2.370998837920489</v>
       </c>
       <c r="N3" t="n">
-        <v>0.7266275906976744</v>
+        <v>0.8814733455657493</v>
       </c>
       <c r="O3" t="n">
-        <v>10.35635074418605</v>
+        <v>10.34508996941896</v>
       </c>
       <c r="P3" t="n">
-        <v>0.7928844651162791</v>
+        <v>0.7743905810397553</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.7548074418604651</v>
+        <v>0.717050764525994</v>
       </c>
       <c r="R3" t="n">
-        <v>0.9114976744186045</v>
+        <v>1.000770642201835</v>
       </c>
       <c r="S3" t="n">
-        <v>2.170746511627907</v>
+        <v>2.352613149847095</v>
       </c>
       <c r="T3" t="n">
-        <v>0.4834418604651163</v>
+        <v>0.5525993883792049</v>
       </c>
       <c r="U3" t="n">
-        <v>0.04005581395348837</v>
+        <v>0.03477675840978593</v>
       </c>
       <c r="V3" t="n">
-        <v>2.484558139534884</v>
+        <v>2.800489296636086</v>
       </c>
       <c r="W3" t="n">
-        <v>15.99426353488372</v>
+        <v>16.8110173088685</v>
       </c>
       <c r="X3" t="n">
-        <v>17.02325953488372</v>
+        <v>15.40909724770642</v>
       </c>
       <c r="Y3" t="n">
-        <v>3.379371162790698</v>
+        <v>3.488552905198777</v>
       </c>
       <c r="Z3" t="n">
-        <v>5.200637488372093</v>
+        <v>5.041825871559633</v>
       </c>
       <c r="AA3" t="n">
-        <v>1.266697674418605</v>
+        <v>1.161590214067278</v>
       </c>
       <c r="AB3" t="n">
-        <v>6.970827906976744</v>
+        <v>7.292960244648319</v>
       </c>
       <c r="AC3" t="n">
-        <v>1.829851162790698</v>
+        <v>1.597284403669725</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.7820465116279071</v>
+        <v>0.783302752293578</v>
       </c>
       <c r="AE3" t="n">
-        <v>3.954976744186047</v>
+        <v>4.839388379204894</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.05023255813953489</v>
+        <v>0.05932721712538226</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.8371162790697674</v>
+        <v>0.8877064220183487</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.1330790697674419</v>
+        <v>0.1068256880733945</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.008372093023255815</v>
+        <v>0.01100917431192661</v>
       </c>
       <c r="AJ3" t="n">
-        <v>4.458232558139535</v>
+        <v>4.972477064220183</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.6930232558139535</v>
+        <v>0.7743119266055046</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.4350697674418604</v>
+        <v>0.36348623853211</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.191706976744186</v>
+        <v>0.2158807339449541</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.1888372093023256</v>
+        <v>0.1920489296636086</v>
       </c>
       <c r="AO3" t="n">
-        <v>1.151162790697674</v>
+        <v>1.004587155963303</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.1944186046511628</v>
+        <v>0.1889908256880734</v>
       </c>
       <c r="AQ3" t="n">
-        <v>2.433209302325581</v>
+        <v>2.147400611620795</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.0827906976744186</v>
+        <v>0.1027522935779817</v>
       </c>
       <c r="AS3" t="n">
-        <v>0.1143255813953488</v>
+        <v>0.09168195718654434</v>
       </c>
       <c r="AT3" t="n">
-        <v>0.02700651162790697</v>
+        <v>0.02081467889908256</v>
       </c>
       <c r="AU3" t="n">
-        <v>0.230495711627907</v>
+        <v>0.2098261651376147</v>
       </c>
       <c r="AV3" t="n">
-        <v>0.3229767441860465</v>
+        <v>0.2123547400611621</v>
       </c>
       <c r="AW3" t="n">
-        <v>0.00372093023255814</v>
+        <v>0.002446483180428134</v>
       </c>
       <c r="AX3" t="n">
-        <v>0.1525581395348837</v>
+        <v>0.1003058103975535</v>
       </c>
       <c r="AY3" t="n">
-        <v>0.1189581395348837</v>
+        <v>0.1399877675840979</v>
       </c>
       <c r="AZ3" t="n">
-        <v>0.06773023255813954</v>
+        <v>0.05655045871559632</v>
       </c>
       <c r="BA3" t="n">
-        <v>0.08837209302325581</v>
+        <v>0.1162079510703364</v>
       </c>
       <c r="BB3" t="n">
-        <v>0.1293023255813953</v>
+        <v>0.1425076452599388</v>
       </c>
       <c r="BC3" t="n">
-        <v>0.1306976744186047</v>
+        <v>0.1241590214067278</v>
       </c>
       <c r="BD3" t="n">
-        <v>0.00186046511627907</v>
+        <v>0.002446483180428134</v>
       </c>
       <c r="BE3" t="n">
-        <v>0.2883720930232558</v>
+        <v>0.1896024464831804</v>
       </c>
       <c r="BF3" t="n">
-        <v>0.1023255813953488</v>
+        <v>0.06727828746177369</v>
       </c>
     </row>
     <row r="4">
@@ -1083,175 +1083,175 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>172.3783641604232</v>
+        <v>170.8015139597039</v>
       </c>
       <c r="C4" t="n">
-        <v>178.2767124234715</v>
+        <v>175.7301977756064</v>
       </c>
       <c r="D4" t="n">
-        <v>264.7416687216495</v>
+        <v>266.2792443884322</v>
       </c>
       <c r="E4" t="n">
-        <v>8.663261756700047</v>
+        <v>7.933057211767471</v>
       </c>
       <c r="F4" t="n">
-        <v>489.427671438406</v>
+        <v>461.7141092721857</v>
       </c>
       <c r="G4" t="n">
-        <v>53.56799375298572</v>
+        <v>55.1643501079648</v>
       </c>
       <c r="H4" t="n">
-        <v>5.576329236187802</v>
+        <v>5.241193937347566</v>
       </c>
       <c r="I4" t="n">
-        <v>14.97693891414395</v>
+        <v>14.43025883318906</v>
       </c>
       <c r="J4" t="n">
-        <v>2.211288483530493</v>
+        <v>2.275768028177686</v>
       </c>
       <c r="K4" t="n">
-        <v>4.103774760985357</v>
+        <v>4.049892237353795</v>
       </c>
       <c r="L4" t="n">
-        <v>4.078796532713496</v>
+        <v>3.860511874647623</v>
       </c>
       <c r="M4" t="n">
-        <v>6.125582072415667</v>
+        <v>6.160563958352327</v>
       </c>
       <c r="N4" t="n">
-        <v>2.646323594591868</v>
+        <v>2.971876882390224</v>
       </c>
       <c r="O4" t="n">
-        <v>23.03866647654552</v>
+        <v>23.1478367038604</v>
       </c>
       <c r="P4" t="n">
-        <v>3.077657893283742</v>
+        <v>3.015764116707798</v>
       </c>
       <c r="Q4" t="n">
-        <v>3.266692017983054</v>
+        <v>3.032049149629505</v>
       </c>
       <c r="R4" t="n">
-        <v>3.981902319106418</v>
+        <v>4.265997727970499</v>
       </c>
       <c r="S4" t="n">
-        <v>7.250421179712024</v>
+        <v>7.656827042114531</v>
       </c>
       <c r="T4" t="n">
-        <v>5.531541962708991</v>
+        <v>5.766733219708937</v>
       </c>
       <c r="U4" t="n">
-        <v>0.7248391567881506</v>
+        <v>0.6795032896421683</v>
       </c>
       <c r="V4" t="n">
-        <v>12.22441552319462</v>
+        <v>13.15255371717166</v>
       </c>
       <c r="W4" t="n">
-        <v>16.58084713488369</v>
+        <v>17.25161803799747</v>
       </c>
       <c r="X4" t="n">
-        <v>23.35975146193549</v>
+        <v>22.3090527511125</v>
       </c>
       <c r="Y4" t="n">
-        <v>9.432285889235903</v>
+        <v>9.690967072405822</v>
       </c>
       <c r="Z4" t="n">
-        <v>7.498241486954451</v>
+        <v>7.579589853608191</v>
       </c>
       <c r="AA4" t="n">
-        <v>5.2584457229822</v>
+        <v>4.962464007956041</v>
       </c>
       <c r="AB4" t="n">
-        <v>17.81100408304223</v>
+        <v>18.27056699063752</v>
       </c>
       <c r="AC4" t="n">
-        <v>6.872994813467096</v>
+        <v>5.853922386648625</v>
       </c>
       <c r="AD4" t="n">
-        <v>4.942262871229881</v>
+        <v>4.923544846826659</v>
       </c>
       <c r="AE4" t="n">
-        <v>14.59881394491225</v>
+        <v>16.12726635062274</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.4645610670003466</v>
+        <v>0.5095449165622132</v>
       </c>
       <c r="AG4" t="n">
-        <v>4.943657323131617</v>
+        <v>5.207913600985133</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.6822526142731546</v>
+        <v>0.6088160075433837</v>
       </c>
       <c r="AI4" t="n">
-        <v>0.2219866520950508</v>
+        <v>0.2544606156837249</v>
       </c>
       <c r="AJ4" t="n">
-        <v>14.44076047101594</v>
+        <v>15.65345214110412</v>
       </c>
       <c r="AK4" t="n">
-        <v>3.670329684756222</v>
+        <v>3.846084109176198</v>
       </c>
       <c r="AL4" t="n">
-        <v>4.620663236246521</v>
+        <v>3.86379090111829</v>
       </c>
       <c r="AM4" t="n">
-        <v>2.56376089343622</v>
+        <v>2.797872145849133</v>
       </c>
       <c r="AN4" t="n">
-        <v>2.572716402849236</v>
+        <v>2.74672349998403</v>
       </c>
       <c r="AO4" t="n">
-        <v>8.331341626782079</v>
+        <v>7.848910440423774</v>
       </c>
       <c r="AP4" t="n">
-        <v>2.785030233233743</v>
+        <v>2.783783455539091</v>
       </c>
       <c r="AQ4" t="n">
-        <v>12.04827287853288</v>
+        <v>11.31317016253348</v>
       </c>
       <c r="AR4" t="n">
-        <v>1.407492463672588</v>
+        <v>1.60757418050475</v>
       </c>
       <c r="AS4" t="n">
-        <v>1.485623027030005</v>
+        <v>1.253442475074843</v>
       </c>
       <c r="AT4" t="n">
-        <v>0.4871925530593037</v>
+        <v>0.4139523938354764</v>
       </c>
       <c r="AU4" t="n">
-        <v>3.122418496156169</v>
+        <v>3.030133417613262</v>
       </c>
       <c r="AV4" t="n">
-        <v>4.313883705027461</v>
+        <v>3.500752711004466</v>
       </c>
       <c r="AW4" t="n">
-        <v>0.08622604802806416</v>
+        <v>0.06992833395269185</v>
       </c>
       <c r="AX4" t="n">
-        <v>2.429064480530276</v>
+        <v>1.970645944572111</v>
       </c>
       <c r="AY4" t="n">
-        <v>2.054837511895867</v>
+        <v>2.338934415099468</v>
       </c>
       <c r="AZ4" t="n">
-        <v>0.8179011278293423</v>
+        <v>0.7467866472862025</v>
       </c>
       <c r="BA4" t="n">
-        <v>2.07328593608727</v>
+        <v>2.376434758185518</v>
       </c>
       <c r="BB4" t="n">
-        <v>2.470124465674896</v>
+        <v>2.604463229532489</v>
       </c>
       <c r="BC4" t="n">
-        <v>2.24477190588382</v>
+        <v>2.387146286275178</v>
       </c>
       <c r="BD4" t="n">
-        <v>0.06099942813304195</v>
+        <v>0.06992833395269185</v>
       </c>
       <c r="BE4" t="n">
-        <v>3.812481297223446</v>
+        <v>3.093921790387864</v>
       </c>
       <c r="BF4" t="n">
-        <v>1.935347996569944</v>
+        <v>1.569795882150027</v>
       </c>
     </row>
     <row r="5">
@@ -1439,25 +1439,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C6" t="n">
         <v>474</v>
       </c>
       <c r="D6" t="n">
-        <v>797</v>
+        <v>777</v>
       </c>
       <c r="E6" t="n">
         <v>2</v>
       </c>
       <c r="F6" t="n">
-        <v>1582</v>
+        <v>1549</v>
       </c>
       <c r="G6" t="n">
-        <v>54.1</v>
+        <v>54.0225</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.375</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -1617,25 +1617,25 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>666.95</v>
+        <v>668</v>
       </c>
       <c r="C7" t="n">
-        <v>730</v>
+        <v>727.2</v>
       </c>
       <c r="D7" t="n">
-        <v>1140</v>
+        <v>1136</v>
       </c>
       <c r="E7" t="n">
         <v>4</v>
       </c>
       <c r="F7" t="n">
-        <v>1745</v>
+        <v>1739</v>
       </c>
       <c r="G7" t="n">
-        <v>88.7</v>
+        <v>86.7</v>
       </c>
       <c r="H7" t="n">
-        <v>1.8</v>
+        <v>1.565</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -1680,7 +1680,7 @@
         <v>0</v>
       </c>
       <c r="W7" t="n">
-        <v>12.5</v>
+        <v>13</v>
       </c>
       <c r="X7" t="n">
         <v>0</v>
@@ -1795,28 +1795,28 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>741.5</v>
+        <v>740</v>
       </c>
       <c r="C8" t="n">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="D8" t="n">
-        <v>1265</v>
+        <v>1251</v>
       </c>
       <c r="E8" t="n">
-        <v>7.125</v>
+        <v>7</v>
       </c>
       <c r="F8" t="n">
-        <v>1872.5</v>
+        <v>1873</v>
       </c>
       <c r="G8" t="n">
-        <v>103</v>
+        <v>102.425</v>
       </c>
       <c r="H8" t="n">
-        <v>5.8</v>
+        <v>5.425000000000001</v>
       </c>
       <c r="I8" t="n">
-        <v>9.75</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
@@ -1858,10 +1858,10 @@
         <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>25</v>
+        <v>27.4</v>
       </c>
       <c r="X8" t="n">
-        <v>41.635</v>
+        <v>36.85</v>
       </c>
       <c r="Y8" t="n">
         <v>0</v>

</xml_diff>